<commit_message>
Fix heading size discrepancy on 2018 sheet
</commit_message>
<xml_diff>
--- a/Ligrarian.xlsx
+++ b/Ligrarian.xlsx
@@ -229,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,10 +326,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,12 +364,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -386,7 +382,7 @@
   <dimension ref="A1:J178"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -451,7 +447,7 @@
       </c>
       <c r="I3" s="15" t="n">
         <f aca="true">(TODAY()-DATE(2018,1,1))/365</f>
-        <v>0.142465753424658</v>
+        <v>0.76986301369863</v>
       </c>
       <c r="J3" s="16"/>
     </row>
@@ -709,22 +705,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -733,15 +729,15 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="25"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="11"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="8" t="s">
         <v>21</v>
       </c>
@@ -749,44 +745,44 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="29"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="15" t="n">
         <f aca="true">(TODAY()-DATE(2018,1,1))/52</f>
-        <v>1</v>
+        <v>5.40384615384615</v>
       </c>
       <c r="J5" s="16" t="n">
         <f aca="false">I5/52</f>
-        <v>0.0192307692307692</v>
+        <v>0.103920118343195</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="29"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="14" t="s">
         <v>8</v>
       </c>
@@ -797,13 +793,13 @@
       <c r="J6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="29"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="14" t="s">
         <v>9</v>
       </c>
@@ -813,17 +809,17 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="11"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="29"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="31" t="e">
+      <c r="I8" s="30" t="e">
         <f aca="false">AVERAGE(C2:C150)</f>
         <v>#DIV/0!</v>
       </c>
@@ -833,8 +829,8 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="29"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="14" t="s">
         <v>13</v>
       </c>
@@ -852,8 +848,8 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="29"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="14" t="s">
         <v>14</v>
       </c>
@@ -871,8 +867,8 @@
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="29"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="14" t="s">
         <v>15</v>
       </c>
@@ -886,8 +882,8 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="14" t="s">
         <v>23</v>
       </c>
@@ -905,8 +901,8 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="14" t="s">
         <v>17</v>
       </c>
@@ -917,13 +913,13 @@
       <c r="J13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="11"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="29"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="14" t="s">
         <v>18</v>
       </c>
@@ -937,9 +933,9 @@
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="29"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="14" t="s">
         <v>19</v>
       </c>
@@ -957,9 +953,9 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="29"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="14" t="s">
         <v>20</v>
       </c>

</xml_diff>